<commit_message>
ajout de la prise en chages des taches necessaires pour executer la tache courante dans Extract_data.py
</commit_message>
<xml_diff>
--- a/data/Sequencement OUEST Modified.xlsx
+++ b/data/Sequencement OUEST Modified.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patri\OneDrive\Cours\PI\livrables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patri\OneDrive\Cours\PI\planificateur\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="350" documentId="11_B662AB16C63DE678B3C5EC32A4B5E48F06B9A5D3" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7ED3C477-AB52-41B6-97B9-C1D396162981}"/>
+  <xr:revisionPtr revIDLastSave="351" documentId="11_B662AB16C63DE678B3C5EC32A4B5E48F06B9A5D3" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5C8E82BB-6C23-49A4-90D6-2061EBF7A047}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="895" firstSheet="47" activeTab="67" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13140" yWindow="1695" windowWidth="7500" windowHeight="6000" tabRatio="895" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MS1-01" sheetId="1" r:id="rId1"/>
@@ -3653,7 +3653,7 @@
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="55" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6234,7 +6234,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -8400,7 +8400,7 @@
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="40" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -10711,7 +10711,7 @@
   <dimension ref="A1:N37"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="40" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -13191,8 +13191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="40" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="40" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -17602,7 +17602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4300-000000000000}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="40" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="40" workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Correction des req de GTW-07 et  de GTW-12 dans Sequencement_OUEST
</commit_message>
<xml_diff>
--- a/data/Sequencement OUEST Modified.xlsx
+++ b/data/Sequencement OUEST Modified.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11213"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paul/Documents/5ir/projet Intégrateur/planificateur/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{931D6554-F185-4C4F-AAA8-245A7803D21F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20BF07F8-7073-564C-BC70-2A0295B62711}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6980" yWindow="1700" windowWidth="16160" windowHeight="13660" tabRatio="895" firstSheet="50" activeTab="55" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15980" yWindow="2220" windowWidth="16160" windowHeight="13660" tabRatio="895" firstSheet="53" activeTab="58" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MS1-01" sheetId="1" r:id="rId1"/>
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1624" uniqueCount="875">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1627" uniqueCount="875">
   <si>
     <t>BWW0001</t>
   </si>
@@ -13815,7 +13815,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="40" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -13831,6 +13831,9 @@
     <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2" s="58" t="s">
         <v>628</v>
+      </c>
+      <c r="B2" t="s">
+        <v>853</v>
       </c>
       <c r="H2" s="57"/>
       <c r="I2" s="57"/>
@@ -14640,8 +14643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3700-000000000000}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="40" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="40" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -15103,7 +15106,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="40" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -15119,6 +15122,9 @@
     <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2" s="54" t="s">
         <v>592</v>
+      </c>
+      <c r="B2" t="s">
+        <v>849</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.15">
@@ -15331,8 +15337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3A00-000000000000}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="40" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="40" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -15348,6 +15354,9 @@
     <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2" s="60" t="s">
         <v>648</v>
+      </c>
+      <c r="B2" t="s">
+        <v>858</v>
       </c>
       <c r="H2" s="60"/>
       <c r="I2" s="1" t="s">
@@ -16413,7 +16422,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3E00-000000000000}">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="40" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScaleNormal="100" zoomScalePageLayoutView="40" workbookViewId="0">
       <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
@@ -17611,7 +17620,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="40" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>

</xml_diff>